<commit_message>
[Added html for inventory item], [updated finding all repairs api]
</commit_message>
<xml_diff>
--- a/04_API/HangarBay.xlsx
+++ b/04_API/HangarBay.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>API planning</t>
   </si>
@@ -156,20 +156,33 @@
 Res: Repair scheduled</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>/repairs/{id}</t>
+    <t>/repairs/all</t>
   </si>
   <si>
     <t>200 OK
 All repairs</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>/repairs</t>
+  </si>
+  <si>
+    <t>cat: [String]</t>
+  </si>
+  <si>
+    <t>200 OK
+All repairs associated with the category array</t>
+  </si>
+  <si>
     <t>7</t>
   </si>
   <si>
     <t>PUT</t>
+  </si>
+  <si>
+    <t>/repairs/{id}</t>
   </si>
   <si>
     <t>status</t>
@@ -188,7 +201,7 @@
     <t>/technician/operator</t>
   </si>
   <si>
-    <t>specializations: String</t>
+    <t>specializations: [String]</t>
   </si>
   <si>
     <t>200 OK
@@ -205,11 +218,21 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="12"/>
@@ -231,11 +254,11 @@
     <font>
       <b val="1"/>
       <sz val="32"/>
-      <color indexed="20"/>
+      <color indexed="23"/>
       <name val="Publico Headline Roman"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -250,13 +273,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -296,11 +313,96 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="20"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -314,7 +416,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -325,7 +427,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -338,7 +440,61 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -347,55 +503,10 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -404,13 +515,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
@@ -419,16 +530,38 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="12"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
         <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -438,93 +571,132 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="10" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="16" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="10" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -544,8 +716,9 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="fffffbef"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffb3afaa"/>
       <rgbColor rgb="ffffd34e"/>
-      <rgbColor rgb="ffb3afaa"/>
       <rgbColor rgb="ffcccac6"/>
       <rgbColor rgb="ffe4e2de"/>
       <rgbColor rgb="ffec6554"/>
@@ -553,8 +726,10 @@
       <rgbColor rgb="ff8bdf7b"/>
       <rgbColor rgb="ff85df57"/>
       <rgbColor rgb="ffb3e095"/>
+      <rgbColor rgb="ff90bf72"/>
+      <rgbColor rgb="ffc19c3b"/>
       <rgbColor rgb="fff0ebe2"/>
-      <rgbColor rgb="ff494a49"/>
+      <rgbColor rgb="ff4a4a4a"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -571,7 +746,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1387346</xdr:colOff>
+      <xdr:colOff>1425446</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>725576</xdr:rowOff>
     </xdr:to>
@@ -582,8 +757,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="-19050" y="-49861"/>
-          <a:ext cx="9274047" cy="725578"/>
+          <a:off x="-19051" y="-47321"/>
+          <a:ext cx="9324848" cy="725578"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -606,7 +781,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="415431" rtl="0" latinLnBrk="0">
+          <a:pPr marL="0" marR="0" indent="0" algn="l" defTabSz="415430" latinLnBrk="0">
             <a:lnSpc>
               <a:spcPct val="100000"/>
             </a:lnSpc>
@@ -625,9 +800,9 @@
                 <a:srgbClr val="4A4A4A"/>
               </a:solidFill>
               <a:uFillTx/>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="Publico Headline Roman"/>
+              <a:ea typeface="Publico Headline Roman"/>
+              <a:cs typeface="Publico Headline Roman"/>
               <a:sym typeface="Publico Headline Roman"/>
             </a:defRPr>
           </a:pPr>
@@ -637,9 +812,9 @@
                 <a:srgbClr val="4A4A4A"/>
               </a:solidFill>
               <a:uFillTx/>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mj-ea"/>
-              <a:cs typeface="+mj-cs"/>
+              <a:latin typeface="Publico Headline Roman"/>
+              <a:ea typeface="Publico Headline Roman"/>
+              <a:cs typeface="Publico Headline Roman"/>
               <a:sym typeface="Publico Headline Roman"/>
             </a:rPr>
             <a:t>HangarBay APIs</a:t>
@@ -654,13 +829,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>647700</xdr:rowOff>
+      <xdr:rowOff>648970</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>201587</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>647700</xdr:rowOff>
+      <xdr:rowOff>648970</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -668,9 +843,9 @@
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="-1" y="647700"/>
-          <a:ext cx="12482489" cy="1"/>
+        <a:xfrm>
+          <a:off x="0" y="648969"/>
+          <a:ext cx="12495188" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -709,10 +884,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="4A4A4B"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="C2C3C6"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="53BBE0"/>
@@ -741,14 +916,14 @@
     </a:clrScheme>
     <a:fontScheme name="26_Meal_Planner">
       <a:majorFont>
-        <a:latin typeface="Publico Headline Roman"/>
-        <a:ea typeface="Publico Headline Roman"/>
-        <a:cs typeface="Publico Headline Roman"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Avenir Next Regular"/>
-        <a:ea typeface="Avenir Next Regular"/>
-        <a:cs typeface="Avenir Next Regular"/>
+        <a:latin typeface="Helvetica Neue"/>
+        <a:ea typeface="Helvetica Neue"/>
+        <a:cs typeface="Helvetica Neue"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="26_Meal_Planner">
@@ -889,11 +1064,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="4B4A4B"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -902,33 +1080,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="all" i="0" spc="0" strike="noStrike" sz="1400" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Publico Text Roman"/>
-            <a:ea typeface="Publico Text Roman"/>
-            <a:cs typeface="Publico Text Roman"/>
-            <a:sym typeface="Publico Text Roman"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Avenir Next Regular"/>
+            <a:ea typeface="Avenir Next Regular"/>
+            <a:cs typeface="Avenir Next Regular"/>
+            <a:sym typeface="Avenir Next Regular"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1167,12 +1345,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1453,12 +1631,12 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="400"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
           </a:spcBef>
           <a:spcAft>
             <a:spcPts val="0"/>
@@ -1476,9 +1654,9 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
+            <a:latin typeface="Avenir Next Regular"/>
+            <a:ea typeface="Avenir Next Regular"/>
+            <a:cs typeface="Avenir Next Regular"/>
             <a:sym typeface="Avenir Next Regular"/>
           </a:defRPr>
         </a:defPPr>
@@ -1721,295 +1899,355 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:H13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.3862" defaultRowHeight="21.65" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="15.3333" defaultRowHeight="21.65" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.7891" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.7422" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.4844" style="1" customWidth="1"/>
-    <col min="4" max="8" width="21.1797" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="15.3906" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="13.8516" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" style="1" customWidth="1"/>
+    <col min="4" max="8" width="21.1719" style="1" customWidth="1"/>
+    <col min="9" max="10" width="15.3516" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="15.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="81" customHeight="1"/>
+    <row r="1" ht="81" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+    </row>
     <row r="2" ht="30" customHeight="1">
-      <c r="A2" t="s" s="2">
+      <c r="A2" t="s" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" ht="22.15" customHeight="1">
-      <c r="A3" t="s" s="3">
+      <c r="A3" t="s" s="9">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="4">
+      <c r="B3" t="s" s="10">
         <v>2</v>
       </c>
-      <c r="C3" t="s" s="4">
+      <c r="C3" t="s" s="10">
         <v>3</v>
       </c>
-      <c r="D3" t="s" s="4">
+      <c r="D3" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="E3" t="s" s="4">
+      <c r="E3" t="s" s="10">
         <v>5</v>
       </c>
-      <c r="F3" t="s" s="4">
+      <c r="F3" t="s" s="10">
         <v>6</v>
       </c>
-      <c r="G3" t="s" s="4">
+      <c r="G3" t="s" s="10">
         <v>7</v>
       </c>
-      <c r="H3" t="s" s="5">
+      <c r="H3" t="s" s="11">
         <v>8</v>
       </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" ht="50.4" customHeight="1" hidden="1">
-      <c r="A4" s="6">
+      <c r="A4" s="13">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" t="s" s="8">
+      <c r="B4" s="14"/>
+      <c r="C4" t="s" s="15">
         <v>9</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="10"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" ht="50.4" customHeight="1">
-      <c r="A5" s="11">
+      <c r="A5" s="18">
         <v>1</v>
       </c>
-      <c r="B5" t="s" s="12">
+      <c r="B5" t="s" s="19">
         <v>10</v>
       </c>
-      <c r="C5" t="s" s="13">
+      <c r="C5" t="s" s="20">
         <v>11</v>
       </c>
-      <c r="D5" t="s" s="13">
+      <c r="D5" t="s" s="20">
         <v>12</v>
       </c>
-      <c r="E5" t="s" s="13">
+      <c r="E5" t="s" s="20">
         <v>13</v>
       </c>
-      <c r="F5" t="s" s="13">
+      <c r="F5" t="s" s="20">
         <v>13</v>
       </c>
-      <c r="G5" t="s" s="13">
+      <c r="G5" t="s" s="20">
         <v>13</v>
       </c>
-      <c r="H5" t="s" s="14">
+      <c r="H5" t="s" s="21">
         <v>14</v>
       </c>
+      <c r="I5" s="12"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" ht="50.4" customHeight="1">
-      <c r="A6" t="s" s="15">
+      <c r="A6" t="s" s="22">
         <v>15</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" t="s" s="17">
+      <c r="B6" s="23"/>
+      <c r="C6" t="s" s="24">
         <v>11</v>
       </c>
-      <c r="D6" t="s" s="17">
+      <c r="D6" t="s" s="24">
         <v>12</v>
       </c>
-      <c r="E6" t="s" s="17">
+      <c r="E6" t="s" s="24">
         <v>16</v>
       </c>
-      <c r="F6" t="s" s="17">
+      <c r="F6" t="s" s="24">
         <v>13</v>
       </c>
-      <c r="G6" t="s" s="17">
+      <c r="G6" t="s" s="24">
         <v>13</v>
       </c>
-      <c r="H6" t="s" s="18">
+      <c r="H6" t="s" s="25">
         <v>17</v>
       </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" ht="50.4" customHeight="1">
-      <c r="A7" t="s" s="15">
+      <c r="A7" t="s" s="22">
         <v>18</v>
       </c>
-      <c r="B7" s="16"/>
-      <c r="C7" t="s" s="19">
+      <c r="B7" s="23"/>
+      <c r="C7" t="s" s="26">
         <v>19</v>
       </c>
-      <c r="D7" t="s" s="19">
+      <c r="D7" t="s" s="26">
         <v>20</v>
       </c>
-      <c r="E7" t="s" s="19">
+      <c r="E7" t="s" s="26">
         <v>13</v>
       </c>
-      <c r="F7" t="s" s="19">
+      <c r="F7" t="s" s="26">
         <v>21</v>
       </c>
-      <c r="G7" t="s" s="19">
+      <c r="G7" t="s" s="26">
         <v>13</v>
       </c>
-      <c r="H7" t="s" s="20">
+      <c r="H7" t="s" s="27">
         <v>22</v>
       </c>
+      <c r="I7" s="12"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" ht="50.4" customHeight="1">
-      <c r="A8" t="s" s="15">
+      <c r="A8" t="s" s="22">
         <v>23</v>
       </c>
-      <c r="B8" t="s" s="12">
+      <c r="B8" t="s" s="19">
         <v>24</v>
       </c>
-      <c r="C8" t="s" s="21">
+      <c r="C8" t="s" s="28">
         <v>11</v>
       </c>
-      <c r="D8" t="s" s="21">
+      <c r="D8" t="s" s="28">
         <v>25</v>
       </c>
-      <c r="E8" t="s" s="21">
+      <c r="E8" t="s" s="28">
         <v>26</v>
       </c>
-      <c r="F8" t="s" s="21">
+      <c r="F8" t="s" s="28">
         <v>13</v>
       </c>
-      <c r="G8" t="s" s="21">
+      <c r="G8" t="s" s="28">
         <v>13</v>
       </c>
-      <c r="H8" t="s" s="22">
+      <c r="H8" t="s" s="29">
         <v>27</v>
       </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" ht="98.55" customHeight="1">
-      <c r="A9" t="s" s="15">
+      <c r="A9" t="s" s="22">
         <v>28</v>
       </c>
-      <c r="B9" t="s" s="12">
+      <c r="B9" t="s" s="19">
         <v>29</v>
       </c>
-      <c r="C9" t="s" s="23">
+      <c r="C9" t="s" s="30">
         <v>19</v>
       </c>
-      <c r="D9" t="s" s="23">
+      <c r="D9" t="s" s="30">
         <v>30</v>
       </c>
-      <c r="E9" t="s" s="23">
+      <c r="E9" t="s" s="30">
         <v>13</v>
       </c>
-      <c r="F9" t="s" s="23">
+      <c r="F9" t="s" s="30">
         <v>31</v>
       </c>
-      <c r="G9" t="s" s="23">
+      <c r="G9" t="s" s="30">
         <v>13</v>
       </c>
-      <c r="H9" t="s" s="24">
+      <c r="H9" t="s" s="31">
         <v>32</v>
       </c>
+      <c r="I9" s="12"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" ht="50.4" customHeight="1">
-      <c r="A10" t="s" s="15">
+      <c r="A10" s="22"/>
+      <c r="B10" s="16"/>
+      <c r="C10" t="s" s="32">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s" s="32">
         <v>33</v>
       </c>
-      <c r="B10" s="16"/>
-      <c r="C10" t="s" s="23">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s" s="23">
+      <c r="E10" t="s" s="32">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s" s="32">
+        <v>13</v>
+      </c>
+      <c r="G10" t="s" s="32">
+        <v>13</v>
+      </c>
+      <c r="H10" t="s" s="33">
         <v>34</v>
       </c>
-      <c r="E10" t="s" s="23">
-        <v>13</v>
-      </c>
-      <c r="F10" t="s" s="23">
-        <v>13</v>
-      </c>
-      <c r="G10" t="s" s="23">
-        <v>13</v>
-      </c>
-      <c r="H10" t="s" s="24">
-        <v>35</v>
-      </c>
+      <c r="I10" s="12"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" ht="50.4" customHeight="1">
-      <c r="A11" t="s" s="15">
+      <c r="A11" t="s" s="22">
+        <v>35</v>
+      </c>
+      <c r="B11" s="23"/>
+      <c r="C11" t="s" s="34">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s" s="34">
         <v>36</v>
       </c>
-      <c r="B11" s="16"/>
-      <c r="C11" t="s" s="23">
+      <c r="E11" t="s" s="34">
         <v>37</v>
       </c>
-      <c r="D11" t="s" s="23">
-        <v>34</v>
-      </c>
-      <c r="E11" t="s" s="23">
+      <c r="F11" t="s" s="34">
         <v>13</v>
       </c>
-      <c r="F11" t="s" s="23">
+      <c r="G11" t="s" s="34">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s" s="35">
         <v>38</v>
       </c>
-      <c r="G11" t="s" s="23">
-        <v>13</v>
-      </c>
-      <c r="H11" t="s" s="24">
-        <v>39</v>
-      </c>
+      <c r="I11" s="12"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" ht="50.4" customHeight="1">
-      <c r="A12" t="s" s="15">
+      <c r="A12" t="s" s="22">
+        <v>39</v>
+      </c>
+      <c r="B12" s="23"/>
+      <c r="C12" t="s" s="30">
         <v>40</v>
       </c>
-      <c r="B12" t="s" s="12">
+      <c r="D12" t="s" s="30">
         <v>41</v>
       </c>
-      <c r="C12" t="s" s="23">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s" s="23">
+      <c r="E12" t="s" s="30">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s" s="30">
         <v>42</v>
       </c>
-      <c r="E12" t="s" s="23">
+      <c r="G12" t="s" s="30">
+        <v>13</v>
+      </c>
+      <c r="H12" t="s" s="31">
         <v>43</v>
       </c>
-      <c r="F12" t="s" s="23">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s" s="23">
-        <v>13</v>
-      </c>
-      <c r="H12" t="s" s="24">
-        <v>44</v>
-      </c>
+      <c r="I12" s="12"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" ht="50.4" customHeight="1">
-      <c r="A13" t="s" s="25">
+      <c r="A13" t="s" s="22">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s" s="19">
         <v>45</v>
       </c>
-      <c r="B13" s="26"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="28"/>
+      <c r="C13" t="s" s="30">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s" s="30">
+        <v>46</v>
+      </c>
+      <c r="E13" t="s" s="30">
+        <v>47</v>
+      </c>
+      <c r="F13" t="s" s="30">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s" s="30">
+        <v>13</v>
+      </c>
+      <c r="H13" t="s" s="31">
+        <v>48</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="14" ht="50.4" customHeight="1">
+      <c r="A14" t="s" s="36">
+        <v>49</v>
+      </c>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="B9:B12"/>
   </mergeCells>
   <pageMargins left="0.416667" right="0.416667" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="landscape" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Avenir Next Regular,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>